<commit_message>
Final changes for the print
</commit_message>
<xml_diff>
--- a/_bookdown_files/tables/impact_1.xlsx
+++ b/_bookdown_files/tables/impact_1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filippochiarello/Dropbox/thesis/thesis_source/_bookdown_files/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709F33D3-625C-9D4F-8FDF-686600AA0B2F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="5020" yWindow="2180" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="150000" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Doc_id</t>
   </si>
   <si>
-    <t>Sentence_id</t>
-  </si>
-  <si>
     <t>Token_id</t>
   </si>
   <si>
@@ -47,9 +45,6 @@
     <t>Xpos</t>
   </si>
   <si>
-    <t>Full_target_group</t>
-  </si>
-  <si>
     <t>Each</t>
   </si>
   <si>
@@ -117,12 +112,15 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>Target_group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -239,6 +237,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -506,21 +507,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -530,332 +536,287 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1855</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
-        <v>1</v>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B7" s="5">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B8" s="5">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B10" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
-        <v>9</v>
+      <c r="C10" s="6">
+        <v>152</v>
       </c>
       <c r="D10" s="6">
         <v>152</v>
       </c>
-      <c r="E10" s="6">
-        <v>152</v>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="5">
+    </row>
+    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="5">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="6" t="s">
+      <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1855</v>
+      </c>
+      <c r="B15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="5">
-        <v>13</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>1855</v>
-      </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
-        <v>14</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>